<commit_message>
Add INSERT INTO `workers`.sql
</commit_message>
<xml_diff>
--- a/Design/Cost.xlsx
+++ b/Design/Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roody\Documents\GitHub\Beggar-Office-Jsp\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudy1\Documents\GitHub\Virtual-Beggar-Servlet\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D57997-9AB6-4CE9-9B9E-724DAB0F49E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CEF8A7-99EA-4CEA-8653-E8A34E197EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="18300" xr2:uid="{CFA388DC-BCBE-4ADA-844D-75964697FDAF}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{CFA388DC-BCBE-4ADA-844D-75964697FDAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
@@ -500,15 +500,14 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="59.90625" customWidth="1"/>
     <col min="2" max="3" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="34.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -687,7 +686,7 @@
         <v>5000000</v>
       </c>
       <c r="G8" s="2">
-        <v>28000000</v>
+        <v>22000000</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="39.5" x14ac:dyDescent="1.1000000000000001">
@@ -758,6 +757,9 @@
     <row r="12" spans="1:7" ht="39.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A12" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="D12" s="2">
+        <v>120000000</v>
       </c>
       <c r="E12" s="2">
         <v>400000000</v>

</xml_diff>

<commit_message>
Add Tireless Mad Scientist
</commit_message>
<xml_diff>
--- a/Design/Cost.xlsx
+++ b/Design/Cost.xlsx
@@ -507,7 +507,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,7 +516,7 @@
     <col min="2" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.453125" customWidth="1"/>
-    <col min="7" max="7" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.5">
@@ -777,7 +777,9 @@
       <c r="F12" s="3">
         <v>2000000000</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="4">
+        <v>48000000000</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">

</xml_diff>